<commit_message>
changes in feature branch
</commit_message>
<xml_diff>
--- a/autotests/metadata/Metadata.xlsx
+++ b/autotests/metadata/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siarhei_Zhamoidzik\0. Self Learning\DQE Mentoring Program\CICD for DQE\repo first_try\cicd-first-try\autotests\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86E0859-59D9-4A4F-A0B7-6FE8944B9E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025038D9-F148-485C-876F-83000E12CF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
     <t>UnitMeasureCode</t>
   </si>
   <si>
-    <t>Title</t>
+    <t>Title2</t>
   </si>
 </sst>
 </file>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update metadata and readme
</commit_message>
<xml_diff>
--- a/autotests/metadata/Metadata.xlsx
+++ b/autotests/metadata/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siarhei_Zhamoidzik\0. Self Learning\DQE Mentoring Program\CICD for DQE\repo first_try\cicd-first-try\autotests\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025038D9-F148-485C-876F-83000E12CF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B48B993-D54A-4ADD-B79D-7427F2640E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
     <t>UnitMeasureCode</t>
   </si>
   <si>
-    <t>Title2</t>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
make change to fail automation test
</commit_message>
<xml_diff>
--- a/autotests/metadata/Metadata.xlsx
+++ b/autotests/metadata/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siarhei_Zhamoidzik\0. Self Learning\DQE Mentoring Program\CICD for DQE\repo first_try\cicd-first-try\autotests\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1725E27-5138-46A7-B679-F09A56EFFEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A840B9-1F63-4A4E-A02C-681965D494E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
     <t>UnitMeasureCode</t>
   </si>
   <si>
-    <t>Title</t>
+    <t>Title2</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
made changes to pass test and add file which should be added to all branches
</commit_message>
<xml_diff>
--- a/autotests/metadata/Metadata.xlsx
+++ b/autotests/metadata/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siarhei_Zhamoidzik\0. Self Learning\DQE Mentoring Program\CICD for DQE\repo first_try\cicd-first-try\autotests\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A840B9-1F63-4A4E-A02C-681965D494E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B902C524-BF69-41A2-A684-1DA0BD35BA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
     <t>UnitMeasureCode</t>
   </si>
   <si>
-    <t>Title2</t>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>